<commit_message>
readme amended. server cloud config yml centralized
</commit_message>
<xml_diff>
--- a/tech-stack.xlsx
+++ b/tech-stack.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Brij kishore Pandey</t>
   </si>
@@ -42,18 +42,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://rockylinux.org/download/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patch Management tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ManageEngine Patch Manager Plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.manageengine.com/patch-management/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.comparitech.com/net-admin/best-linux-patch-management-tools/</t>
   </si>
   <si>
     <t xml:space="preserve">K8 Management tool</t>
@@ -198,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,10 +197,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -280,10 +264,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,94 +297,79 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" display="https://rockylinux.org/download/"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://www.manageengine.com/patch-management/"/>
-    <hyperlink ref="D2" r:id="rId3" display="https://www.comparitech.com/net-admin/best-linux-patch-management-tools/"/>
-    <hyperlink ref="C3" r:id="rId4" display="https://ranchermanager.docs.rancher.com/v2.6"/>
-    <hyperlink ref="C4" r:id="rId5" display="https://bazel.build/about/intro"/>
-    <hyperlink ref="C5" r:id="rId6" display="https://buildkite.com/home"/>
-    <hyperlink ref="C6" r:id="rId7" display="https://snyk.io"/>
-    <hyperlink ref="C7" r:id="rId8" display="https://spinnaker.io"/>
-    <hyperlink ref="C8" r:id="rId9" display="https://sematext.com/pricing/"/>
-    <hyperlink ref="D8" r:id="rId10" display="https://sematext.com/blog/cloud-monitoring-tools/"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://ranchermanager.docs.rancher.com/v2.6"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://bazel.build/about/intro"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://buildkite.com/home"/>
+    <hyperlink ref="C5" r:id="rId5" display="https://snyk.io"/>
+    <hyperlink ref="C6" r:id="rId6" display="https://spinnaker.io"/>
+    <hyperlink ref="C7" r:id="rId7" display="https://sematext.com/pricing/"/>
+    <hyperlink ref="D7" r:id="rId8" display="https://sematext.com/blog/cloud-monitoring-tools/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>